<commit_message>
Update site data files
</commit_message>
<xml_diff>
--- a/data/Burrows_2008/raw/site_data.xlsx
+++ b/data/Burrows_2008/raw/site_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208613_ad_unsw_edu_au/Documents/RA Work/AusTraits/austraits.build/data/Burrows_2008/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_F25DC773A252ABDACC10484FF9DC7E805ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CA9CCB4-9016-47F8-B6E3-41BAF7FEE616}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_F25DC773A252ABDACC10484FF9DC7E805ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12275F08-AAB0-426E-B025-A936D58EF92A}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="0" windowWidth="13920" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,25 +30,10 @@
     <t>location_name</t>
   </si>
   <si>
-    <t>vegetation_description</t>
-  </si>
-  <si>
-    <t>soils_and_landform</t>
-  </si>
-  <si>
     <t>climate</t>
   </si>
   <si>
     <t>McCorkhill forest</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>location_notes</t>
   </si>
   <si>
     <t>Lindsay forest</t>
@@ -129,6 +114,21 @@
   </si>
   <si>
     <t>Mediterranean-type climate with cool wet winters and mild summers. Mean annual rainfall varies across the park from 1200-1300 mm.</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>soils and landform</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>longitude (deg)</t>
+  </si>
+  <si>
+    <t>latitude (deg)</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,27 +467,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>115.542</v>
@@ -496,21 +496,21 @@
         <v>-33.957000000000001</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>115.967</v>
@@ -519,21 +519,21 @@
         <v>-34.243000000000002</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>116.617</v>
@@ -542,21 +542,21 @@
         <v>-34.192999999999998</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>116.803</v>
@@ -565,16 +565,16 @@
         <v>-34.987000000000002</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>